<commit_message>
restauration almost done #1
</commit_message>
<xml_diff>
--- a/input/parameter_scenarios.xlsx
+++ b/input/parameter_scenarios.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="42">
   <si>
     <t xml:space="preserve">scenario</t>
   </si>
@@ -38,9 +38,6 @@
   </si>
   <si>
     <t xml:space="preserve">restoration_rate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.01</t>
   </si>
   <si>
     <t xml:space="preserve">0.015</t>
@@ -252,11 +249,11 @@
   </sheetPr>
   <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I18" activeCellId="0" sqref="I18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="256" zoomScaleNormal="256" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.7421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="0" width="12.41"/>
@@ -299,26 +296,26 @@
       <c r="B2" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D2" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="E2" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="0" t="s">
-        <v>8</v>
-      </c>
       <c r="F2" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H2" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -326,25 +323,25 @@
         <v>4</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D3" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="F3" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="0" t="s">
-        <v>15</v>
-      </c>
       <c r="G3" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I3" s="0" t="n">
         <v>0</v>
@@ -355,25 +352,25 @@
         <v>4</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I4" s="0" t="n">
         <v>0</v>
@@ -384,25 +381,25 @@
         <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I5" s="0" t="n">
         <v>0</v>
@@ -413,25 +410,25 @@
         <v>4</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I6" s="0" t="n">
         <v>0</v>
@@ -442,25 +439,25 @@
         <v>4</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I7" s="0" t="n">
         <v>0.3</v>
@@ -471,25 +468,25 @@
         <v>4</v>
       </c>
       <c r="B8" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="0" t="s">
-        <v>21</v>
-      </c>
       <c r="D8" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I8" s="0" t="n">
         <v>0</v>
@@ -500,25 +497,25 @@
         <v>4</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I9" s="0" t="n">
         <v>0</v>
@@ -529,25 +526,25 @@
         <v>4</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I10" s="0" t="n">
         <v>0</v>
@@ -558,25 +555,25 @@
         <v>4</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I11" s="0" t="n">
         <v>0</v>
@@ -587,25 +584,25 @@
         <v>4</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I12" s="0" t="n">
         <v>0</v>
@@ -616,25 +613,25 @@
         <v>4</v>
       </c>
       <c r="B13" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="0" t="s">
+      <c r="D13" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="E13" s="0" t="s">
+      <c r="F13" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="F13" s="0" t="s">
-        <v>29</v>
-      </c>
       <c r="G13" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I13" s="0" t="n">
         <v>0</v>
@@ -645,25 +642,25 @@
         <v>4</v>
       </c>
       <c r="B14" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="D14" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E14" s="0" t="s">
-        <v>31</v>
-      </c>
       <c r="F14" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I14" s="0" t="n">
         <v>0</v>
@@ -674,25 +671,25 @@
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I15" s="0" t="n">
         <v>0</v>
@@ -703,25 +700,25 @@
         <v>4</v>
       </c>
       <c r="B16" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="C16" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="D16" s="0" t="s">
-        <v>34</v>
-      </c>
       <c r="E16" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="F16" s="0" t="s">
-        <v>15</v>
-      </c>
       <c r="G16" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I16" s="0" t="n">
         <v>0</v>
@@ -732,25 +729,25 @@
         <v>4</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I17" s="0" t="n">
         <v>0</v>
@@ -761,7 +758,7 @@
         <v>4</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C18" s="0" t="n">
         <v>45.8</v>
@@ -779,65 +776,65 @@
         <v>33</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I18" s="0" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B19" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="C19" s="0" t="s">
-        <v>6</v>
+      <c r="C19" s="0" t="n">
+        <v>0.5</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E19" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="F19" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="G19" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="H19" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="I19" s="0" t="s">
         <v>39</v>
-      </c>
-      <c r="F19" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="G19" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="H19" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="I19" s="0" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E20" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="F20" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="F20" s="0" t="s">
-        <v>42</v>
-      </c>
       <c r="G20" s="0" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H20" s="0" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I20" s="0" t="n">
         <v>0.5</v>
@@ -845,28 +842,28 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H21" s="0" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I21" s="0" t="n">
         <v>0</v>
@@ -874,28 +871,28 @@
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H22" s="0" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I22" s="0" t="n">
         <v>0</v>
@@ -903,28 +900,28 @@
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H23" s="0" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I23" s="0" t="n">
         <v>0</v>
@@ -932,28 +929,28 @@
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H24" s="0" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I24" s="0" t="n">
         <v>0</v>
@@ -961,28 +958,28 @@
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B25" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C25" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="C25" s="0" t="s">
-        <v>21</v>
-      </c>
       <c r="D25" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G25" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H25" s="0" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I25" s="0" t="n">
         <v>0</v>
@@ -990,28 +987,28 @@
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G26" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H26" s="0" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I26" s="0" t="n">
         <v>0</v>
@@ -1019,28 +1016,28 @@
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G27" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H27" s="0" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I27" s="0" t="n">
         <v>0</v>
@@ -1048,28 +1045,28 @@
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G28" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H28" s="0" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I28" s="0" t="n">
         <v>0</v>
@@ -1077,28 +1074,28 @@
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G29" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H29" s="0" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I29" s="0" t="n">
         <v>0</v>
@@ -1106,28 +1103,28 @@
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B30" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C30" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="C30" s="0" t="s">
+      <c r="D30" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="E30" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="D30" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="E30" s="0" t="s">
+      <c r="F30" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="F30" s="0" t="s">
-        <v>29</v>
-      </c>
       <c r="G30" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H30" s="0" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I30" s="0" t="n">
         <v>0</v>
@@ -1135,28 +1132,28 @@
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B31" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C31" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D31" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E31" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="C31" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="D31" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E31" s="0" t="s">
-        <v>31</v>
-      </c>
       <c r="F31" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G31" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H31" s="0" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I31" s="0" t="n">
         <v>0</v>
@@ -1164,28 +1161,28 @@
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G32" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H32" s="0" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I32" s="0" t="n">
         <v>0</v>
@@ -1193,28 +1190,28 @@
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B33" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="C33" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D33" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="C33" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="D33" s="0" t="s">
-        <v>34</v>
-      </c>
       <c r="E33" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="F33" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="F33" s="0" t="s">
-        <v>15</v>
-      </c>
       <c r="G33" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H33" s="0" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I33" s="0" t="n">
         <v>0</v>
@@ -1222,28 +1219,28 @@
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G34" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H34" s="0" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I34" s="0" t="n">
         <v>0</v>
@@ -1251,10 +1248,10 @@
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C35" s="0" t="n">
         <v>46</v>
@@ -1272,7 +1269,7 @@
         <v>33</v>
       </c>
       <c r="H35" s="0" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I35" s="0" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
added restauration and demolition methods
</commit_message>
<xml_diff>
--- a/input/parameter_scenarios.xlsx
+++ b/input/parameter_scenarios.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="41">
   <si>
     <t xml:space="preserve">scenario</t>
   </si>
@@ -47,9 +47,6 @@
   </si>
   <si>
     <t xml:space="preserve">linear</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.7, 0.8, 1, 0.4</t>
   </si>
   <si>
     <t xml:space="preserve">restoration_deep_amb</t>
@@ -253,7 +250,7 @@
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.76953125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.78515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="0" width="12.41"/>
@@ -297,7 +294,7 @@
         <v>5</v>
       </c>
       <c r="C2" s="0" t="n">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="D2" s="0" t="s">
         <v>6</v>
@@ -314,8 +311,8 @@
       <c r="H2" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="1" t="s">
-        <v>9</v>
+      <c r="I2" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -323,22 +320,22 @@
         <v>4</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D3" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="F3" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="0" t="s">
-        <v>14</v>
-      </c>
       <c r="G3" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H3" s="0" t="s">
         <v>8</v>
@@ -352,22 +349,22 @@
         <v>4</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H4" s="0" t="s">
         <v>8</v>
@@ -381,22 +378,22 @@
         <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H5" s="0" t="s">
         <v>8</v>
@@ -410,22 +407,22 @@
         <v>4</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H6" s="0" t="s">
         <v>8</v>
@@ -439,28 +436,28 @@
         <v>4</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H7" s="0" t="s">
         <v>8</v>
       </c>
       <c r="I7" s="0" t="n">
-        <v>0.3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -468,22 +465,22 @@
         <v>4</v>
       </c>
       <c r="B8" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D8" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" s="0" t="s">
-        <v>20</v>
-      </c>
       <c r="E8" s="0" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H8" s="0" t="s">
         <v>8</v>
@@ -497,22 +494,22 @@
         <v>4</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H9" s="0" t="s">
         <v>8</v>
@@ -526,22 +523,22 @@
         <v>4</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H10" s="0" t="s">
         <v>8</v>
@@ -555,22 +552,22 @@
         <v>4</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H11" s="0" t="s">
         <v>8</v>
@@ -584,22 +581,22 @@
         <v>4</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H12" s="0" t="s">
         <v>8</v>
@@ -613,22 +610,22 @@
         <v>4</v>
       </c>
       <c r="B13" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="0" t="s">
+      <c r="D13" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="D13" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="E13" s="0" t="s">
+      <c r="F13" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="F13" s="0" t="s">
-        <v>28</v>
-      </c>
       <c r="G13" s="0" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H13" s="0" t="s">
         <v>8</v>
@@ -642,22 +639,22 @@
         <v>4</v>
       </c>
       <c r="B14" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="C14" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="D14" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="E14" s="0" t="s">
-        <v>30</v>
-      </c>
       <c r="F14" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H14" s="0" t="s">
         <v>8</v>
@@ -671,22 +668,22 @@
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H15" s="0" t="s">
         <v>8</v>
@@ -700,22 +697,22 @@
         <v>4</v>
       </c>
       <c r="B16" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="D16" s="0" t="s">
-        <v>33</v>
-      </c>
       <c r="E16" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F16" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="F16" s="0" t="s">
-        <v>14</v>
-      </c>
       <c r="G16" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H16" s="0" t="s">
         <v>8</v>
@@ -729,22 +726,22 @@
         <v>4</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H17" s="0" t="s">
         <v>8</v>
@@ -758,7 +755,7 @@
         <v>4</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C18" s="0" t="n">
         <v>45.8</v>
@@ -779,12 +776,12 @@
         <v>8</v>
       </c>
       <c r="I18" s="0" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B19" s="0" t="s">
         <v>5</v>
@@ -796,42 +793,42 @@
         <v>7</v>
       </c>
       <c r="E19" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="F19" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="G19" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="H19" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="I19" s="0" t="s">
         <v>38</v>
-      </c>
-      <c r="F19" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="G19" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="H19" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="I19" s="0" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E20" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="F20" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="F20" s="0" t="s">
-        <v>41</v>
-      </c>
       <c r="G20" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H20" s="0" t="s">
         <v>8</v>
@@ -842,25 +839,25 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H21" s="0" t="s">
         <v>8</v>
@@ -871,25 +868,25 @@
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H22" s="0" t="s">
         <v>8</v>
@@ -900,25 +897,25 @@
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H23" s="0" t="s">
         <v>8</v>
@@ -929,25 +926,25 @@
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H24" s="0" t="s">
         <v>8</v>
@@ -958,25 +955,25 @@
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B25" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C25" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="C25" s="0" t="s">
-        <v>20</v>
-      </c>
       <c r="D25" s="0" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G25" s="0" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H25" s="0" t="s">
         <v>8</v>
@@ -987,25 +984,25 @@
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G26" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H26" s="0" t="s">
         <v>8</v>
@@ -1016,25 +1013,25 @@
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G27" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H27" s="0" t="s">
         <v>8</v>
@@ -1045,25 +1042,25 @@
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G28" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H28" s="0" t="s">
         <v>8</v>
@@ -1074,25 +1071,25 @@
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G29" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H29" s="0" t="s">
         <v>8</v>
@@ -1103,25 +1100,25 @@
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B30" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C30" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="C30" s="0" t="s">
+      <c r="D30" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="E30" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="D30" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="E30" s="0" t="s">
+      <c r="F30" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="F30" s="0" t="s">
-        <v>28</v>
-      </c>
       <c r="G30" s="0" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H30" s="0" t="s">
         <v>8</v>
@@ -1132,25 +1129,25 @@
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B31" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="C31" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D31" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E31" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="C31" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="D31" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="E31" s="0" t="s">
-        <v>30</v>
-      </c>
       <c r="F31" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G31" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H31" s="0" t="s">
         <v>8</v>
@@ -1161,25 +1158,25 @@
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G32" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H32" s="0" t="s">
         <v>8</v>
@@ -1190,25 +1187,25 @@
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B33" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C33" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D33" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="C33" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="D33" s="0" t="s">
-        <v>33</v>
-      </c>
       <c r="E33" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F33" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="F33" s="0" t="s">
-        <v>14</v>
-      </c>
       <c r="G33" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H33" s="0" t="s">
         <v>8</v>
@@ -1219,25 +1216,25 @@
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G34" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H34" s="0" t="s">
         <v>8</v>
@@ -1248,10 +1245,10 @@
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C35" s="0" t="n">
         <v>46</v>

</xml_diff>